<commit_message>
Commit after changing excel data
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533990\Downloads\dotnet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533990\Documents\44663\MVC-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>ACS+2</t>
   </si>
@@ -179,93 +179,9 @@
     <t>Summer 2018</t>
   </si>
   <si>
-    <t>S533991</t>
-  </si>
-  <si>
-    <t>S533992</t>
-  </si>
-  <si>
-    <t>S533993</t>
-  </si>
-  <si>
-    <t>S533994</t>
-  </si>
-  <si>
     <t>Summer Off</t>
   </si>
   <si>
-    <t>S511111</t>
-  </si>
-  <si>
-    <t>S511112</t>
-  </si>
-  <si>
-    <t>S511113</t>
-  </si>
-  <si>
-    <t>S511114</t>
-  </si>
-  <si>
-    <t>S511115</t>
-  </si>
-  <si>
-    <t>S511116</t>
-  </si>
-  <si>
-    <t>S511117</t>
-  </si>
-  <si>
-    <t>S511118</t>
-  </si>
-  <si>
-    <t>Man</t>
-  </si>
-  <si>
-    <t>Can</t>
-  </si>
-  <si>
-    <t>Tan</t>
-  </si>
-  <si>
-    <t>Chan</t>
-  </si>
-  <si>
-    <t>Flan</t>
-  </si>
-  <si>
-    <t>Clan</t>
-  </si>
-  <si>
-    <t>Tlan</t>
-  </si>
-  <si>
-    <t>Mlan</t>
-  </si>
-  <si>
-    <t>Bun</t>
-  </si>
-  <si>
-    <t>Hyn</t>
-  </si>
-  <si>
-    <t>Sus</t>
-  </si>
-  <si>
-    <t>Chin</t>
-  </si>
-  <si>
-    <t>Kin</t>
-  </si>
-  <si>
-    <t>Jlin</t>
-  </si>
-  <si>
-    <t>Fin</t>
-  </si>
-  <si>
-    <t>Flin</t>
-  </si>
-  <si>
     <t>DegreeID(PK)</t>
   </si>
   <si>
@@ -296,10 +212,49 @@
     <t>StudentID(PK)</t>
   </si>
   <si>
-    <t>StudentId(PK)</t>
-  </si>
-  <si>
     <t>TermID(FK)</t>
+  </si>
+  <si>
+    <t>S531366</t>
+  </si>
+  <si>
+    <t>S533710</t>
+  </si>
+  <si>
+    <t>S533626</t>
+  </si>
+  <si>
+    <t>S531383</t>
+  </si>
+  <si>
+    <t>Hari Priya</t>
+  </si>
+  <si>
+    <t>Jupally</t>
+  </si>
+  <si>
+    <t>Bharadwaj</t>
+  </si>
+  <si>
+    <t>Dasari</t>
+  </si>
+  <si>
+    <t>Durga Susmitha</t>
+  </si>
+  <si>
+    <t>Kotyada</t>
+  </si>
+  <si>
+    <t>Hyndavi</t>
+  </si>
+  <si>
+    <t>Musipatla</t>
+  </si>
+  <si>
+    <t>Vyshnavi</t>
+  </si>
+  <si>
+    <t>Yalamareddy</t>
   </si>
 </sst>
 </file>
@@ -629,7 +584,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -702,7 +657,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -876,13 +831,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1435,13 +1390,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2507,10 +2462,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,13 +2478,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
         <v>36</v>
@@ -2540,13 +2495,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>38</v>
@@ -2557,19 +2512,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2580,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -2597,24 +2552,24 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -2625,30 +2580,30 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>38</v>
@@ -2659,19 +2614,53 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2681,9 +2670,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2696,7 +2687,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -2710,114 +2701,60 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D2">
-        <v>919534873</v>
+        <v>919569151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3">
-        <v>919534873</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4">
-        <v>919534873</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5">
-        <v>919534873</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>74</v>
-      </c>
-      <c r="D6">
-        <v>919534873</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7">
-        <v>919534873</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8">
-        <v>919534873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9">
-        <v>919534873</v>
       </c>
     </row>
   </sheetData>
@@ -2830,7 +2767,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,10 +2777,10 @@
         <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
         <v>43</v>
@@ -2868,7 +2805,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2882,7 +2819,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2896,7 +2833,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2910,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>5</v>

</xml_diff>

<commit_message>
Commit some more changes in the excel data
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>ACS+2</t>
   </si>
@@ -149,12 +149,6 @@
     <t>No Summer Off</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
     <t>S533990</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>TermID(PK)</t>
   </si>
   <si>
-    <t>RequuirementID(FK)</t>
-  </si>
-  <si>
     <t>StudentID(FK)</t>
   </si>
   <si>
@@ -255,19 +246,32 @@
   </si>
   <si>
     <t>Yalamareddy</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,8 +294,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +579,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -582,14 +589,14 @@
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -646,7 +653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -655,14 +664,14 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -819,7 +828,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,15 +838,15 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1378,7 +1387,7 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,15 +1397,15 @@
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2464,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,20 +2485,20 @@
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2501,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>38</v>
@@ -2518,13 +2527,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2535,7 +2544,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -2552,13 +2561,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -2586,13 +2595,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
         <v>38</v>
@@ -2620,13 +2629,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2637,7 +2646,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -2654,13 +2663,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2682,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,79 +2695,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1">
         <v>919</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
+      <c r="A2">
+        <v>533990</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2">
         <v>919569151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>61</v>
+      <c r="A3">
+        <v>531366</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>919559663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>533710</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4">
+        <v>919570698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>533626</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5">
+        <v>919570835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>531383</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
+      <c r="D6">
+        <v>919562271</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2766,94 +2788,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
+      <c r="B2">
+        <v>533990</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
+      <c r="B3">
+        <v>531366</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
+      <c r="B4">
+        <v>533710</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>63</v>
+      <c r="B5">
+        <v>533626</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>64</v>
+      <c r="B6">
+        <v>531383</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed changes to Student class in models and Dbinitializer.cs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
     <t>MS ACS + DB</t>
   </si>
   <si>
-    <t>DegreeAbbrev(U, max 6)</t>
-  </si>
-  <si>
-    <t>DegreeName(U, max 20)</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>Summer Off</t>
   </si>
   <si>
-    <t>DegreeID(PK)</t>
-  </si>
-  <si>
     <t>RequirementID(PK)</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>StudentID(FK)</t>
   </si>
   <si>
-    <t>StudentID(PK)</t>
-  </si>
-  <si>
     <t>TermID(FK)</t>
   </si>
   <si>
@@ -222,6 +210,18 @@
   </si>
   <si>
     <t>str</t>
+  </si>
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>DegreeID</t>
+  </si>
+  <si>
+    <t>DegreeAbbrev</t>
+  </si>
+  <si>
+    <t>DegreeName</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -563,19 +563,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -589,11 +589,11 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"='"&amp;B2&amp;"', "&amp;$C$1&amp;"='"&amp;C2&amp;"'},"</f>
-        <v>new Degree{DegreeID(PK)=2, DegreeAbbrev(U, max 6)='ACS+DB', DegreeName(U, max 20)='MS ACS + DB'},</v>
+        <v>new Degree{DegreeID=2, DegreeAbbrev='ACS+DB', DegreeName='MS ACS + DB'},</v>
       </c>
     </row>
   </sheetData>
@@ -618,13 +618,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,10 +632,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,10 +643,10 @@
         <v>542</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,10 +654,10 @@
         <v>563</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,10 +665,10 @@
         <v>560</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,10 +676,10 @@
         <v>555</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,10 +687,10 @@
         <v>618</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,10 +709,10 @@
         <v>664</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,10 +720,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,10 +731,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,10 +742,10 @@
         <v>691</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,10 +753,10 @@
         <v>692</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -781,13 +781,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,13 +944,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,19 +1239,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,10 +1265,10 @@
         <v>533990</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,10 +1282,10 @@
         <v>533990</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,10 +1299,10 @@
         <v>531366</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1316,10 +1316,10 @@
         <v>531366</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1333,10 +1333,10 @@
         <v>533710</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1350,10 +1350,10 @@
         <v>533710</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1367,10 +1367,10 @@
         <v>533626</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,10 +1384,10 @@
         <v>533626</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,10 +1401,10 @@
         <v>531383</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,10 +1418,10 @@
         <v>531383</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1431,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,91 +1443,111 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="86.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1">
         <v>919</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>533990</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>919569151</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="str">
+        <f>CONCATENATE("new Student{","StudentID=",A:A,",","FirstName=''",B:B,"''",",","LastName=''",C:C,"''",",",,,"919=",D:D,,"}",",")</f>
+        <v>new Student{StudentID=533990,FirstName=''Hari Priya'',LastName=''Jupally'',919=919569151},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>531366</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>919559663</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E6" si="0">CONCATENATE("new Student{","StudentID=",A:A,",","FirstName=''",B:B,"''",",","LastName=''",C:C,"''",",",,,"919=",D:D,,"}",",")</f>
+        <v>new Student{StudentID=531366,FirstName=''Bharadwaj'',LastName=''Dasari'',919=919559663},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>533710</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>919570698</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentID=533710,FirstName=''Durga Susmitha'',LastName=''Kotyada'',919=919570698},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>533626</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>919570835</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentID=533626,FirstName=''Hyndavi'',LastName=''Musipatla'',919=919570835},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>531383</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>919562271</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentID=531383,FirstName=''Vyshnavi'',LastName=''Yalamareddy'',919=919562271},</v>
       </c>
     </row>
   </sheetData>
@@ -1554,16 +1574,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,7 +1653,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1661,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +1695,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1689,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1703,7 +1723,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1731,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,7 +1779,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,7 +1793,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1815,7 +1835,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1849,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,7 +1933,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commited changes in Models, Added new DegreeRequirement.cs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533990\Documents\44663\MVC-Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531366\Documents\44663\MVC-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>ACS+DB</t>
   </si>
@@ -146,9 +146,6 @@
     <t>RequirementID(PK)</t>
   </si>
   <si>
-    <t>DegreeRequirementID(PK)</t>
-  </si>
-  <si>
     <t>DegreeID(FK)</t>
   </si>
   <si>
@@ -222,6 +219,12 @@
   </si>
   <si>
     <t>DegreeName</t>
+  </si>
+  <si>
+    <t>RequirementID</t>
+  </si>
+  <si>
+    <t>DegreeRequirementID</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -563,19 +566,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -589,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"='"&amp;B2&amp;"', "&amp;$C$1&amp;"='"&amp;C2&amp;"'},"</f>
@@ -766,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,20 +780,21 @@
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="81.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -800,8 +804,12 @@
       <c r="C2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=1,DegreeID=2,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -811,8 +819,12 @@
       <c r="C3">
         <v>542</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=2,DegreeID=2,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -822,8 +834,12 @@
       <c r="C4">
         <v>563</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=3,DegreeID=2,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -833,8 +849,12 @@
       <c r="C5">
         <v>560</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=4,DegreeID=2,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -844,8 +864,12 @@
       <c r="C6">
         <v>555</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=5,DegreeID=2,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -855,8 +879,12 @@
       <c r="C7">
         <v>618</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=6,DegreeID=2,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -866,8 +894,12 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=7,DegreeID=2,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -877,8 +909,12 @@
       <c r="C9">
         <v>664</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=8,DegreeID=2,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -888,8 +924,12 @@
       <c r="C10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=9,DegreeID=2,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -899,8 +939,12 @@
       <c r="C11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=10,DegreeID=2,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -910,8 +954,12 @@
       <c r="C12">
         <v>691</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=11,DegreeID=2,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -920,6 +968,10 @@
       </c>
       <c r="C13">
         <v>692</v>
+      </c>
+      <c r="D13" t="str">
+        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreeRequirement{DegreeRequirementID=12,DegreeID=2,RequirementID=692},</v>
       </c>
     </row>
   </sheetData>
@@ -944,13 +996,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,13 +1291,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>26</v>
@@ -1448,13 +1500,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D1" s="1">
         <v>919</v>
@@ -1465,10 +1517,10 @@
         <v>533990</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
       <c r="D2">
         <v>919569151</v>
@@ -1483,10 +1535,10 @@
         <v>531366</v>
       </c>
       <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
       </c>
       <c r="D3">
         <v>919559663</v>
@@ -1501,10 +1553,10 @@
         <v>533710</v>
       </c>
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
       </c>
       <c r="D4">
         <v>919570698</v>
@@ -1519,10 +1571,10 @@
         <v>533626</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
       </c>
       <c r="D5">
         <v>919570835</v>
@@ -1537,10 +1589,10 @@
         <v>531383</v>
       </c>
       <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
       </c>
       <c r="D6">
         <v>919562271</v>
@@ -1577,10 +1629,10 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Commited changes to DegreePlan.cs in Model
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531366\Documents\44663\MVC-Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533626\Documents\44663\MVC-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>GDP2</t>
   </si>
   <si>
-    <t>DegreePlanAbbrev(U, 8)</t>
-  </si>
-  <si>
-    <t>DegreePlanName(U, 20)</t>
-  </si>
-  <si>
     <t>No Summer Off</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>RequirementID(PK)</t>
   </si>
   <si>
-    <t>DegreeID(FK)</t>
-  </si>
-  <si>
     <t>RequirementID(FK)</t>
   </si>
   <si>
@@ -225,6 +216,15 @@
   </si>
   <si>
     <t>DegreeRequirementID</t>
+  </si>
+  <si>
+    <t>DegreePlanID</t>
+  </si>
+  <si>
+    <t>DegreePlanAbbrev</t>
+  </si>
+  <si>
+    <t>DegreePlanName</t>
   </si>
 </sst>
 </file>
@@ -566,19 +566,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"='"&amp;B2&amp;"', "&amp;$C$1&amp;"='"&amp;C2&amp;"'},"</f>
@@ -621,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,13 +785,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>460</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" ref="D2:D13" si="0">CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
         <v>new DegreeRequirement{DegreeRequirementID=1,DegreeID=2,RequirementID=460},</v>
       </c>
     </row>
@@ -820,7 +820,7 @@
         <v>542</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=2,DegreeID=2,RequirementID=542},</v>
       </c>
     </row>
@@ -835,7 +835,7 @@
         <v>563</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=3,DegreeID=2,RequirementID=563},</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>560</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=4,DegreeID=2,RequirementID=560},</v>
       </c>
     </row>
@@ -865,7 +865,7 @@
         <v>555</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=5,DegreeID=2,RequirementID=555},</v>
       </c>
     </row>
@@ -880,7 +880,7 @@
         <v>618</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=6,DegreeID=2,RequirementID=618},</v>
       </c>
     </row>
@@ -895,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=7,DegreeID=2,RequirementID=1},</v>
       </c>
     </row>
@@ -910,7 +910,7 @@
         <v>664</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=8,DegreeID=2,RequirementID=664},</v>
       </c>
     </row>
@@ -925,7 +925,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=9,DegreeID=2,RequirementID=10},</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
         <v>20</v>
       </c>
       <c r="D11" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=10,DegreeID=2,RequirementID=20},</v>
       </c>
     </row>
@@ -955,7 +955,7 @@
         <v>691</v>
       </c>
       <c r="D12" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=11,DegreeID=2,RequirementID=691},</v>
       </c>
     </row>
@@ -970,7 +970,7 @@
         <v>692</v>
       </c>
       <c r="D13" t="str">
-        <f>CONCATENATE("new DegreeRequirement{","DegreeRequirementID=",A:A,",","DegreeID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <f t="shared" si="0"/>
         <v>new DegreeRequirement{DegreeRequirementID=12,DegreeID=2,RequirementID=692},</v>
       </c>
     </row>
@@ -996,13 +996,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1276,9 +1276,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1287,26 +1289,27 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="131.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1317,13 +1320,17 @@
         <v>533990</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE("new DegreePlan{","DegreePlanID=",A:A,",","DegreeID=",B:B,",","StudentID=",C:C,",","DegreePlanAbbrev=","''",D:D,"''",",","DegreePlanName=","''",E:E,"''","},")</f>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
@@ -1334,13 +1341,17 @@
         <v>533990</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F11" si="0">CONCATENATE("new DegreePlan{","DegreePlanID=",A:A,",","DegreeID=",B:B,",","StudentID=",C:C,",","DegreePlanAbbrev=","''",D:D,"''",",","DegreePlanName=","''",E:E,"''","},")</f>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -1351,13 +1362,17 @@
         <v>531366</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -1368,13 +1383,17 @@
         <v>531366</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1385,13 +1404,17 @@
         <v>533710</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -1402,13 +1425,17 @@
         <v>533710</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -1419,13 +1446,17 @@
         <v>533626</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -1436,13 +1467,17 @@
         <v>533626</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1453,13 +1488,17 @@
         <v>531383</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -1470,10 +1509,14 @@
         <v>531383</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
   </sheetData>
@@ -1500,13 +1543,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1">
         <v>919</v>
@@ -1517,10 +1560,10 @@
         <v>533990</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>919569151</v>
@@ -1535,10 +1578,10 @@
         <v>531366</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>919559663</v>
@@ -1553,10 +1596,10 @@
         <v>533710</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>919570698</v>
@@ -1571,10 +1614,10 @@
         <v>533626</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>919570835</v>
@@ -1589,10 +1632,10 @@
         <v>531383</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>919562271</v>
@@ -1626,16 +1669,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1663,7 +1706,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,7 +1720,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1691,7 +1734,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1719,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1733,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1761,7 +1804,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,7 +1846,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1860,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,7 +1874,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1845,7 +1888,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1859,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,7 +1916,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,7 +1930,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,7 +1944,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1929,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1943,7 +1986,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1957,7 +2000,7 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,7 +2014,7 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +2028,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commited changes in DegreePlanTermRequirement.cs in Model and updated Dbinitializer.cs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533626\Documents\44663\MVC-Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531383\Documents\44663\New MVC\MVC-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CD17BE-7B9C-42A9-8F3B-DADF5494D075}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -20,17 +21,22 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>ACS+DB</t>
   </si>
@@ -140,21 +146,12 @@
     <t>RequirementID(PK)</t>
   </si>
   <si>
-    <t>RequirementID(FK)</t>
-  </si>
-  <si>
-    <t>DegreePlanID(PK)</t>
-  </si>
-  <si>
     <t>TermID(PK)</t>
   </si>
   <si>
     <t>StudentID(FK)</t>
   </si>
   <si>
-    <t>TermID(FK)</t>
-  </si>
-  <si>
     <t>Hari Priya</t>
   </si>
   <si>
@@ -225,12 +222,15 @@
   </si>
   <si>
     <t>DegreePlanName</t>
+  </si>
+  <si>
+    <t>TermID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -566,19 +566,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"='"&amp;B2&amp;"', "&amp;$C$1&amp;"='"&amp;C2&amp;"'},"</f>
@@ -605,7 +605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -768,7 +768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -785,13 +785,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,11 +980,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,20 +992,21 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="77.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1015,8 +1016,12 @@
       <c r="C2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>CONCATENATE("new DegreePlanTermRequirement{","DegreePlanID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -1026,8 +1031,12 @@
       <c r="C3">
         <v>542</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D25" si="0">CONCATENATE("new DegreePlanTermRequirement{","DegreePlanID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -1037,8 +1046,12 @@
       <c r="C4">
         <v>563</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
@@ -1048,8 +1061,12 @@
       <c r="C5">
         <v>560</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -1059,8 +1076,12 @@
       <c r="C6">
         <v>555</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -1070,8 +1091,12 @@
       <c r="C7">
         <v>618</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -1081,8 +1106,12 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1092,8 +1121,12 @@
       <c r="C9">
         <v>664</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1103,8 +1136,12 @@
       <c r="C10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -1114,8 +1151,12 @@
       <c r="C11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1125,8 +1166,12 @@
       <c r="C12">
         <v>691</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1136,8 +1181,12 @@
       <c r="C13">
         <v>692</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=692},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1147,8 +1196,12 @@
       <c r="C14">
         <v>460</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=460},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1158,8 +1211,12 @@
       <c r="C15">
         <v>542</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=542},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1169,8 +1226,12 @@
       <c r="C16">
         <v>563</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=563},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1180,8 +1241,12 @@
       <c r="C17">
         <v>560</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=560},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1191,8 +1256,12 @@
       <c r="C18">
         <v>555</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=555},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1202,8 +1271,12 @@
       <c r="C19">
         <v>618</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=618},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1213,8 +1286,12 @@
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=1},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1224,8 +1301,12 @@
       <c r="C21">
         <v>664</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=664},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1235,8 +1316,12 @@
       <c r="C22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=10},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1246,8 +1331,12 @@
       <c r="C23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=20},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -1257,8 +1346,12 @@
       <c r="C24">
         <v>691</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=691},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1267,6 +1360,10 @@
       </c>
       <c r="C25">
         <v>692</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=692},</v>
       </c>
     </row>
   </sheetData>
@@ -1275,11 +1372,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,19 +1391,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,7 +1622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1543,13 +1640,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1">
         <v>919</v>
@@ -1560,10 +1657,10 @@
         <v>533990</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>919569151</v>
@@ -1578,10 +1675,10 @@
         <v>531366</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>919559663</v>
@@ -1596,10 +1693,10 @@
         <v>533710</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>919570698</v>
@@ -1614,10 +1711,10 @@
         <v>533626</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>919570835</v>
@@ -1632,10 +1729,10 @@
         <v>531383</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>919562271</v>
@@ -1652,7 +1749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1672,10 +1769,10 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Commit after Data Seeding.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531383\Documents\MVC-Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533990\Documents\44663\MVC-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F337130C-D8C1-432D-86F8-56A12BF3E686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>ACS+DB</t>
   </si>
@@ -225,12 +224,15 @@
   </si>
   <si>
     <t>TermID</t>
+  </si>
+  <si>
+    <t>DegreePlanTermRequirementID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -605,7 +607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -768,7 +770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -980,24 +982,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" customWidth="1"/>
+    <col min="4" max="4" width="101.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>62</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1017,13 +1017,13 @@
         <v>460</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("new DegreePlanTermRequirement{","DegreePlanID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=460},</v>
+        <f>CONCATENATE("new DegreePlanTermRequirement{","DegreePlanTermRequirementID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=1,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1032,13 +1032,13 @@
         <v>542</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D25" si="0">CONCATENATE("new DegreePlanTermRequirement{","DegreePlanID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=542},</v>
+        <f t="shared" ref="D3:D25" si="0">CONCATENATE("new DegreePlanTermRequirement{","DegreePlanTermRequirementID=",A:A,",","TermID=",B:B,",","RequirementID=",C:C,"},")</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=2,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1048,12 +1048,12 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=1,RequirementID=563},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=3,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1063,12 +1063,12 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=560},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=4,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1078,12 +1078,12 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=555},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=5,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1093,12 +1093,12 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=2,RequirementID=618},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=6,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1108,12 +1108,12 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=1},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=7,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1123,12 +1123,12 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=664},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=8,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=3,RequirementID=10},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=9,TermID=3,RequirementID=10},</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -1153,12 +1153,12 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=20},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=10,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=691},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=11,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=12,TermID=4,RequirementID=692},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=12,TermID=4,RequirementID=692},</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=460},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=13,TermID=1,RequirementID=460},</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1213,12 +1213,12 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=542},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=14,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1228,12 +1228,12 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=1,RequirementID=563},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1243,12 +1243,12 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=560},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=16,TermID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1258,12 +1258,12 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=555},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=17,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1273,12 +1273,12 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=2,RequirementID=618},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=18,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1288,12 +1288,12 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=1},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=19,TermID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1303,12 +1303,12 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=664},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=20,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1318,12 +1318,12 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=4,RequirementID=10},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=21,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -1333,12 +1333,12 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=20},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=22,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -1348,12 +1348,12 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=691},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=23,TermID=5,RequirementID=691},</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlanTermRequirement{DegreePlanID=13,TermID=5,RequirementID=692},</v>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=24,TermID=5,RequirementID=692},</v>
       </c>
     </row>
   </sheetData>
@@ -1372,11 +1372,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1424,12 +1424,12 @@
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE("new DegreePlan{","DegreePlanID=",A:A,",","DegreeID=",B:B,",","StudentID=",C:C,",","DegreePlanAbbrev=","''",D:D,"''",",","DegreePlanName=","''",E:E,"''","},")</f>
-        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=1,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1445,12 +1445,12 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F11" si="0">CONCATENATE("new DegreePlan{","DegreePlanID=",A:A,",","DegreeID=",B:B,",","StudentID=",C:C,",","DegreePlanAbbrev=","''",D:D,"''",",","DegreePlanName=","''",E:E,"''","},")</f>
-        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=2,DegreeID=2,StudentID=533990,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1466,12 +1466,12 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=3,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1487,12 +1487,12 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=4,DegreeID=2,StudentID=531366,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1508,12 +1508,12 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=5,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=6,DegreeID=2,StudentID=533710,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1550,12 +1550,12 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=7,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1571,12 +1571,12 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=8,DegreeID=2,StudentID=533626,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1592,12 +1592,12 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=12,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=9,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''No Summer Off'',DegreePlanName=''No Summer Off''},</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=13,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
+        <v>new DegreePlan{DegreePlanID=10,DegreeID=2,StudentID=531383,DegreePlanAbbrev=''Summer Off'',DegreePlanName=''Summer Off''},</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1749,11 +1749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>531366</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>531366</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>531366</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>531366</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>531366</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>533710</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>533710</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>533710</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>533710</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>533710</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>533626</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>533626</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>533626</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>533626</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>533626</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>531383</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>531383</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>531383</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>531383</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>531383</v>

</xml_diff>